<commit_message>
Updated spreadsheet for emotional timeline
</commit_message>
<xml_diff>
--- a/planning/timelinevshappiness.xlsx
+++ b/planning/timelinevshappiness.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10833"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10833" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Happiness" sheetId="2" r:id="rId1"/>
@@ -3979,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4862,8 +4862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>